<commit_message>
Validação de erros em progresso
</commit_message>
<xml_diff>
--- a/src/frontend/components/sheets/Lista_Exemplo.xlsx
+++ b/src/frontend/components/sheets/Lista_Exemplo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="EstaPasta_de_trabalho" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrey\Desktop\Nova pasta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\AndreyOliveira0\LeitorArquivos-Vue\src\frontend\components\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -448,14 +448,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -741,14 +748,14 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.28515625" customWidth="1"/>
     <col min="2" max="2" width="25.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="5" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" customWidth="1"/>
     <col min="6" max="6" width="16.140625" customWidth="1"/>
@@ -793,7 +800,7 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -825,7 +832,7 @@
       <c r="B2" t="s">
         <v>30</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="5">
         <v>1</v>
       </c>
       <c r="D2" s="2">
@@ -857,7 +864,7 @@
       <c r="B3" t="s">
         <v>39</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="5">
         <v>2</v>
       </c>
       <c r="D3" s="2">
@@ -889,7 +896,7 @@
       <c r="B4" t="s">
         <v>40</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="5">
         <v>3</v>
       </c>
       <c r="D4" s="2">
@@ -921,7 +928,7 @@
       <c r="B5" t="s">
         <v>43</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="5">
         <v>4</v>
       </c>
       <c r="D5" s="2">
@@ -953,7 +960,7 @@
       <c r="B6" t="s">
         <v>41</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="5">
         <v>5</v>
       </c>
       <c r="D6" s="2">
@@ -985,7 +992,7 @@
       <c r="B7" t="s">
         <v>42</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="5">
         <v>6</v>
       </c>
       <c r="D7" s="2">
@@ -1017,7 +1024,7 @@
       <c r="B8" t="s">
         <v>44</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="5">
         <v>7</v>
       </c>
       <c r="D8" s="2">
@@ -1043,7 +1050,7 @@
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="3"/>
+      <c r="C18" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1057,7 +1064,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1077,7 +1084,7 @@
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1461,13 +1468,13 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="5" customWidth="1"/>
     <col min="3" max="3" width="28.140625" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" customWidth="1"/>
     <col min="5" max="5" width="28.28515625" customWidth="1"/>
@@ -1481,7 +1488,7 @@
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1499,7 +1506,7 @@
       <c r="G1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>15</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -1510,10 +1517,10 @@
       <c r="A2" t="s">
         <v>92</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="5">
         <v>20251234</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>93</v>
       </c>
       <c r="D2" t="s">
@@ -1539,10 +1546,10 @@
       <c r="A3" t="s">
         <v>96</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="5">
         <v>20255789</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>97</v>
       </c>
       <c r="D3" t="s">
@@ -1568,10 +1575,10 @@
       <c r="A4" t="s">
         <v>100</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="5">
         <v>20249876</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>102</v>
       </c>
       <c r="D4" t="s">
@@ -1597,10 +1604,10 @@
       <c r="A5" t="s">
         <v>106</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="5">
         <v>20254985</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>107</v>
       </c>
       <c r="D5" t="s">
@@ -1626,10 +1633,10 @@
       <c r="A6" t="s">
         <v>109</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="5">
         <v>20236254</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>111</v>
       </c>
       <c r="D6" t="s">
@@ -1655,10 +1662,10 @@
       <c r="A7" t="s">
         <v>115</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="5">
         <v>20232565</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>114</v>
       </c>
       <c r="D7" t="s">
@@ -1699,7 +1706,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1719,7 +1726,7 @@
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1737,7 +1744,7 @@
       <c r="G1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="7" t="s">
         <v>18</v>
       </c>
       <c r="I1" s="1" t="s">

</xml_diff>

<commit_message>
Popups e mensagens de erros
</commit_message>
<xml_diff>
--- a/src/frontend/components/sheets/Lista_Exemplo.xlsx
+++ b/src/frontend/components/sheets/Lista_Exemplo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Disciplinas" sheetId="1" r:id="rId1"/>
@@ -299,9 +299,6 @@
     <t>Roberto Teixeira</t>
   </si>
   <si>
-    <t>Prof. Leticia Barros</t>
-  </si>
-  <si>
     <t>Biologia Celular</t>
   </si>
   <si>
@@ -381,6 +378,9 @@
   </si>
   <si>
     <t>Estagiario</t>
+  </si>
+  <si>
+    <t>Leticia Barros</t>
   </si>
 </sst>
 </file>
@@ -747,7 +747,7 @@
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -1063,8 +1063,8 @@
   <sheetPr codeName="Planilha2"/>
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1436,7 +1436,7 @@
         <v>65</v>
       </c>
       <c r="C13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D13" t="s">
         <v>71</v>
@@ -1451,7 +1451,7 @@
         <v>45836</v>
       </c>
       <c r="H13" t="s">
-        <v>90</v>
+        <v>117</v>
       </c>
       <c r="I13" t="s">
         <v>74</v>
@@ -1515,19 +1515,19 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" s="5">
         <v>20251234</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" t="s">
         <v>93</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>94</v>
-      </c>
-      <c r="E2" t="s">
-        <v>95</v>
       </c>
       <c r="F2" s="2">
         <v>37684</v>
@@ -1536,7 +1536,7 @@
         <v>45836</v>
       </c>
       <c r="H2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I2" t="s">
         <v>33</v>
@@ -1544,19 +1544,19 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B3" s="5">
         <v>20255789</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F3" s="2">
         <v>38300</v>
@@ -1565,27 +1565,27 @@
         <v>45832</v>
       </c>
       <c r="H3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B4" s="5">
         <v>20249876</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" t="s">
         <v>94</v>
-      </c>
-      <c r="E4" t="s">
-        <v>95</v>
       </c>
       <c r="F4" s="2">
         <v>37156</v>
@@ -1594,27 +1594,27 @@
         <v>45360</v>
       </c>
       <c r="H4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B5" s="5">
         <v>20254985</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F5" s="2">
         <v>33257</v>
@@ -1623,7 +1623,7 @@
         <v>45839</v>
       </c>
       <c r="H5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I5" t="s">
         <v>33</v>
@@ -1631,16 +1631,16 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B6" s="5">
         <v>20236254</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E6" t="s">
         <v>40</v>
@@ -1652,7 +1652,7 @@
         <v>44959</v>
       </c>
       <c r="H6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I6" t="s">
         <v>33</v>
@@ -1660,16 +1660,16 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B7" s="5">
         <v>20232565</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E7" t="s">
         <v>44</v>
@@ -1681,7 +1681,7 @@
         <v>45269</v>
       </c>
       <c r="H7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I7" t="s">
         <v>33</v>
@@ -1753,7 +1753,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2">
         <v>20251234</v>
@@ -1762,10 +1762,10 @@
         <v>48</v>
       </c>
       <c r="D2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F2" s="2">
         <v>45720</v>
@@ -1782,7 +1782,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3">
         <v>20236254</v>
@@ -1794,7 +1794,7 @@
         <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F3" s="2">
         <v>45716</v>
@@ -1811,7 +1811,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B4">
         <v>20232565</v>
@@ -1823,7 +1823,7 @@
         <v>44</v>
       </c>
       <c r="E4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F4" s="2">
         <v>45116</v>
@@ -1835,7 +1835,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tentativa de executar o service do frontend
</commit_message>
<xml_diff>
--- a/src/frontend/components/sheets/Lista_Exemplo.xlsx
+++ b/src/frontend/components/sheets/Lista_Exemplo.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="EstaPasta_de_trabalho" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <workbookPr codeName="EstaPasta_de_trabalho"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\AndreyOliveira0\LeitorArquivos-Vue\src\frontend\components\sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caioh\OneDrive\Documentos\GitHub\LeitorArquivos-Vue\src\frontend\components\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E50176C-9828-4290-BCDC-687976CC540F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Disciplinas" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="131">
   <si>
     <t>Disciplina</t>
   </si>
@@ -182,9 +183,6 @@
     <t>Turma B</t>
   </si>
   <si>
-    <t>T001</t>
-  </si>
-  <si>
     <t>Calculo I</t>
   </si>
   <si>
@@ -194,39 +192,6 @@
     <t>Ricardo Luiz</t>
   </si>
   <si>
-    <t>T002</t>
-  </si>
-  <si>
-    <t>T003</t>
-  </si>
-  <si>
-    <t>T004</t>
-  </si>
-  <si>
-    <t>T005</t>
-  </si>
-  <si>
-    <t>T006</t>
-  </si>
-  <si>
-    <t>T007</t>
-  </si>
-  <si>
-    <t>T008</t>
-  </si>
-  <si>
-    <t>T009</t>
-  </si>
-  <si>
-    <t>T010</t>
-  </si>
-  <si>
-    <t>T011</t>
-  </si>
-  <si>
-    <t>T012</t>
-  </si>
-  <si>
     <t>Fisica I</t>
   </si>
   <si>
@@ -381,13 +346,88 @@
   </si>
   <si>
     <t>Leticia Barros</t>
+  </si>
+  <si>
+    <t>T013</t>
+  </si>
+  <si>
+    <t>T014</t>
+  </si>
+  <si>
+    <t>T015</t>
+  </si>
+  <si>
+    <t>T016</t>
+  </si>
+  <si>
+    <t>T017</t>
+  </si>
+  <si>
+    <t>T018</t>
+  </si>
+  <si>
+    <t>T019</t>
+  </si>
+  <si>
+    <t>T020</t>
+  </si>
+  <si>
+    <t>T021</t>
+  </si>
+  <si>
+    <t>T022</t>
+  </si>
+  <si>
+    <t>T023</t>
+  </si>
+  <si>
+    <t>T024</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>20251853</t>
+  </si>
+  <si>
+    <t>20255832</t>
+  </si>
+  <si>
+    <t>20249245</t>
+  </si>
+  <si>
+    <t>20254321</t>
+  </si>
+  <si>
+    <t>20236123</t>
+  </si>
+  <si>
+    <t>20232935</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -407,6 +447,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -459,10 +507,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -743,12 +791,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Planilha1"/>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,8 +880,8 @@
       <c r="B2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="5">
-        <v>1</v>
+      <c r="C2" s="5" t="s">
+        <v>118</v>
       </c>
       <c r="D2" s="2">
         <v>45698</v>
@@ -864,8 +912,8 @@
       <c r="B3" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="5">
-        <v>2</v>
+      <c r="C3" s="5" t="s">
+        <v>119</v>
       </c>
       <c r="D3" s="2">
         <v>45698</v>
@@ -896,8 +944,8 @@
       <c r="B4" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="5">
-        <v>3</v>
+      <c r="C4" s="5" t="s">
+        <v>120</v>
       </c>
       <c r="D4" s="2">
         <v>45698</v>
@@ -928,8 +976,8 @@
       <c r="B5" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="5">
-        <v>4</v>
+      <c r="C5" s="5" t="s">
+        <v>121</v>
       </c>
       <c r="D5" s="2">
         <v>45705</v>
@@ -960,8 +1008,8 @@
       <c r="B6" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="5">
-        <v>5</v>
+      <c r="C6" s="5" t="s">
+        <v>122</v>
       </c>
       <c r="D6" s="2">
         <v>45700</v>
@@ -992,8 +1040,8 @@
       <c r="B7" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="5">
-        <v>6</v>
+      <c r="C7" s="5" t="s">
+        <v>123</v>
       </c>
       <c r="D7" s="2">
         <v>45703</v>
@@ -1024,8 +1072,8 @@
       <c r="B8" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="5">
-        <v>7</v>
+      <c r="C8" s="5" t="s">
+        <v>124</v>
       </c>
       <c r="D8" s="2">
         <v>45699</v>
@@ -1049,8 +1097,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="6"/>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D12" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1059,12 +1107,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Planilha2"/>
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1114,13 +1162,13 @@
         <v>46</v>
       </c>
       <c r="B2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" t="s">
         <v>51</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>52</v>
-      </c>
-      <c r="D2" t="s">
-        <v>53</v>
       </c>
       <c r="E2">
         <v>40</v>
@@ -1132,7 +1180,7 @@
         <v>45836</v>
       </c>
       <c r="H2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I2" t="s">
         <v>33</v>
@@ -1143,13 +1191,13 @@
         <v>47</v>
       </c>
       <c r="B3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" t="s">
         <v>55</v>
-      </c>
-      <c r="C3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" t="s">
-        <v>67</v>
       </c>
       <c r="E3">
         <v>35</v>
@@ -1161,10 +1209,10 @@
         <v>45836</v>
       </c>
       <c r="H3" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="I3" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1172,13 +1220,13 @@
         <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>108</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="E4">
         <v>30</v>
@@ -1190,7 +1238,7 @@
         <v>45836</v>
       </c>
       <c r="H4" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="I4" t="s">
         <v>33</v>
@@ -1201,13 +1249,13 @@
         <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="C5" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="D5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E5">
         <v>40</v>
@@ -1219,10 +1267,10 @@
         <v>45836</v>
       </c>
       <c r="H5" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="I5" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1230,13 +1278,13 @@
         <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>110</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="D6" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E6">
         <v>25</v>
@@ -1248,10 +1296,10 @@
         <v>45836</v>
       </c>
       <c r="H6" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="I6" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1259,13 +1307,13 @@
         <v>50</v>
       </c>
       <c r="B7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" t="s">
         <v>59</v>
-      </c>
-      <c r="C7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" t="s">
-        <v>71</v>
       </c>
       <c r="E7">
         <v>35</v>
@@ -1277,7 +1325,7 @@
         <v>45836</v>
       </c>
       <c r="H7" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="I7" t="s">
         <v>33</v>
@@ -1288,13 +1336,13 @@
         <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>112</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E8">
         <v>45</v>
@@ -1306,10 +1354,10 @@
         <v>45836</v>
       </c>
       <c r="H8" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="I8" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1317,13 +1365,13 @@
         <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>113</v>
       </c>
       <c r="C9" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="D9" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E9">
         <v>40</v>
@@ -1335,7 +1383,7 @@
         <v>45836</v>
       </c>
       <c r="H9" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="I9" t="s">
         <v>33</v>
@@ -1346,13 +1394,13 @@
         <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>114</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="D10" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="E10">
         <v>30</v>
@@ -1364,10 +1412,10 @@
         <v>45836</v>
       </c>
       <c r="H10" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="I10" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1375,13 +1423,13 @@
         <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>115</v>
       </c>
       <c r="C11" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E11">
         <v>50</v>
@@ -1393,7 +1441,7 @@
         <v>45836</v>
       </c>
       <c r="H11" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="I11" t="s">
         <v>33</v>
@@ -1404,13 +1452,13 @@
         <v>46</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>116</v>
       </c>
       <c r="C12" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="D12" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="E12">
         <v>38</v>
@@ -1422,10 +1470,10 @@
         <v>45836</v>
       </c>
       <c r="H12" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="I12" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1433,13 +1481,13 @@
         <v>50</v>
       </c>
       <c r="B13" t="s">
-        <v>65</v>
+        <v>117</v>
       </c>
       <c r="C13" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="D13" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="E13">
         <v>32</v>
@@ -1451,10 +1499,10 @@
         <v>45836</v>
       </c>
       <c r="H13" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="I13" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1463,12 +1511,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Planilha3"/>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1515,19 +1563,19 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="5">
-        <v>20251234</v>
+        <v>79</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>125</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="D2" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="E2" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="F2" s="2">
         <v>37684</v>
@@ -1536,7 +1584,7 @@
         <v>45836</v>
       </c>
       <c r="H2" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="I2" t="s">
         <v>33</v>
@@ -1544,19 +1592,19 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B3" s="5">
-        <v>20255789</v>
+        <v>83</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>126</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="E3" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="F3" s="2">
         <v>38300</v>
@@ -1565,27 +1613,27 @@
         <v>45832</v>
       </c>
       <c r="H3" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="I3" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B4" s="5">
-        <v>20249876</v>
+        <v>87</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>127</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="D4" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="E4" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="F4" s="2">
         <v>37156</v>
@@ -1594,27 +1642,27 @@
         <v>45360</v>
       </c>
       <c r="H4" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="I4" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B5" s="5">
-        <v>20254985</v>
+        <v>93</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>128</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="D5" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="E5" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="F5" s="2">
         <v>33257</v>
@@ -1623,7 +1671,7 @@
         <v>45839</v>
       </c>
       <c r="H5" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="I5" t="s">
         <v>33</v>
@@ -1631,16 +1679,16 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>108</v>
-      </c>
-      <c r="B6" s="5">
-        <v>20236254</v>
+        <v>96</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>129</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="D6" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="E6" t="s">
         <v>40</v>
@@ -1652,7 +1700,7 @@
         <v>44959</v>
       </c>
       <c r="H6" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="I6" t="s">
         <v>33</v>
@@ -1660,16 +1708,16 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B7" s="5">
-        <v>20232565</v>
+        <v>102</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>130</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="D7" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="E7" t="s">
         <v>44</v>
@@ -1681,32 +1729,35 @@
         <v>45269</v>
       </c>
       <c r="H7" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="I7" t="s">
         <v>33</v>
       </c>
     </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C11" s="7"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
-    <hyperlink ref="C7" r:id="rId6"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Planilha4"/>
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1744,7 +1795,7 @@
       <c r="G1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>18</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -1753,19 +1804,19 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B2">
-        <v>20251234</v>
+        <v>20251853</v>
       </c>
       <c r="C2" t="s">
         <v>48</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="E2" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="F2" s="2">
         <v>45720</v>
@@ -1782,10 +1833,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="B3">
-        <v>20236254</v>
+        <v>20236123</v>
       </c>
       <c r="C3" t="s">
         <v>50</v>
@@ -1794,7 +1845,7 @@
         <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="F3" s="2">
         <v>45716</v>
@@ -1811,10 +1862,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="B4">
-        <v>20232565</v>
+        <v>20232935</v>
       </c>
       <c r="C4" t="s">
         <v>50</v>
@@ -1823,7 +1874,7 @@
         <v>44</v>
       </c>
       <c r="E4" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="F4" s="2">
         <v>45116</v>
@@ -1835,7 +1886,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>